<commit_message>
listo cambios a bd
</commit_message>
<xml_diff>
--- a/database/2control produccion limpio.xlsx
+++ b/database/2control produccion limpio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\mar\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBB944B-5DF8-4141-BB74-482B733FCE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AA0980-77D3-4964-ADFD-9A7D7017355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="3615" windowWidth="24750" windowHeight="10560" xr2:uid="{FD61990A-8B6B-462D-9144-365D0A908497}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="29160" windowHeight="15840" xr2:uid="{FD61990A-8B6B-462D-9144-365D0A908497}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -5982,7 +5982,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5998,13 +5998,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -6016,16 +6040,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6360,8 +6390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A763E7-769D-4CEB-944C-B914C6D40DF1}">
   <dimension ref="A1:I1571"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1554" workbookViewId="0">
-      <selection activeCell="A1571" sqref="A1571"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6389,10 +6419,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">

</xml_diff>